<commit_message>
post-first draft Nature, pre-Vanessa chat
</commit_message>
<xml_diff>
--- a/fWHR/Bastrop scoring.xlsx
+++ b/fWHR/Bastrop scoring.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/VWilson/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s1229179\GitHub\R\fWHR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="660" yWindow="560" windowWidth="24960" windowHeight="13960" tabRatio="500"/>
+    <workbookView xWindow="660" yWindow="555" windowWidth="24960" windowHeight="13965" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="74">
   <si>
     <t>Agreeableness</t>
   </si>
@@ -210,6 +207,45 @@
   </si>
   <si>
     <t>Conscientiousness?</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>6E</t>
+  </si>
+  <si>
+    <t>6C</t>
+  </si>
+  <si>
+    <t>8D</t>
+  </si>
+  <si>
+    <t>3N</t>
+  </si>
+  <si>
+    <t>2A</t>
+  </si>
+  <si>
+    <t>2O</t>
   </si>
 </sst>
 </file>
@@ -301,6 +337,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -569,24 +608,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E43" sqref="E43"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="3" width="13.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.625" customWidth="1"/>
+    <col min="2" max="2" width="15.625" customWidth="1"/>
+    <col min="3" max="3" width="9.875" customWidth="1"/>
+    <col min="4" max="4" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="9.625" customWidth="1"/>
+    <col min="6" max="6" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
@@ -600,7 +641,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -616,8 +657,14 @@
       <c r="E2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -633,8 +680,14 @@
       <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -650,8 +703,14 @@
       <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -667,8 +726,14 @@
       <c r="E5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>62</v>
+      </c>
+      <c r="G5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -684,8 +749,14 @@
       <c r="E6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -701,8 +772,14 @@
       <c r="E7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -712,8 +789,11 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -729,8 +809,11 @@
       <c r="E9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -746,8 +829,11 @@
       <c r="E10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -763,8 +849,11 @@
       <c r="E11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -774,8 +863,11 @@
       <c r="C12" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -788,8 +880,11 @@
       <c r="D13" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -805,8 +900,11 @@
       <c r="E14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -822,8 +920,11 @@
       <c r="E15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -839,8 +940,11 @@
       <c r="E16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -856,8 +960,11 @@
       <c r="E17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -870,8 +977,11 @@
       <c r="D18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -887,8 +997,11 @@
       <c r="E19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -904,8 +1017,11 @@
       <c r="E20" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -918,8 +1034,11 @@
       <c r="D21" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -935,8 +1054,11 @@
       <c r="E22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -952,8 +1074,11 @@
       <c r="E23" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -969,8 +1094,11 @@
       <c r="E24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -986,8 +1114,11 @@
       <c r="E25" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1003,8 +1134,11 @@
       <c r="E26" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -1020,8 +1154,11 @@
       <c r="E27" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1037,8 +1174,11 @@
       <c r="E28" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1048,8 +1188,11 @@
       <c r="C29" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -1059,8 +1202,11 @@
       <c r="C30" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -1076,8 +1222,11 @@
       <c r="E31" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>47</v>
       </c>
@@ -1093,8 +1242,11 @@
       <c r="E32" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>48</v>
       </c>
@@ -1104,8 +1256,11 @@
       <c r="E33" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -1121,8 +1276,11 @@
       <c r="E34" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -1138,8 +1296,11 @@
       <c r="E35" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -1149,8 +1310,11 @@
       <c r="C36" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -1160,8 +1324,11 @@
       <c r="C37" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -1177,8 +1344,11 @@
       <c r="E38" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>54</v>
       </c>
@@ -1194,8 +1364,11 @@
       <c r="E39" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -1211,8 +1384,11 @@
       <c r="E40" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>56</v>
       </c>
@@ -1228,8 +1404,11 @@
       <c r="E41" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>57</v>
       </c>
@@ -1245,8 +1424,12 @@
       <c r="E42" t="s">
         <v>16</v>
       </c>
+      <c r="F42" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
too many changes to describe
see logs
</commit_message>
<xml_diff>
--- a/fWHR/Bastrop scoring.xlsx
+++ b/fWHR/Bastrop scoring.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="75">
   <si>
     <t>Agreeableness</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>2O</t>
+  </si>
+  <si>
+    <t>POS</t>
   </si>
 </sst>
 </file>
@@ -614,7 +617,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -977,6 +980,9 @@
       <c r="D18" t="s">
         <v>30</v>
       </c>
+      <c r="E18" t="s">
+        <v>74</v>
+      </c>
       <c r="F18" t="s">
         <v>64</v>
       </c>

</xml_diff>